<commit_message>
Merged PR 16333: BP-4967 : Inventory Export - News/Non News: Label columns as Rate Card provid...
BP-4967 : Inventory Export - News/Non News: Label columns as Rate Card provided and System Calculated
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Open Market inventory.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Open Market inventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F22E8F-966B-4FE1-AA3A-558C2C674A52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451363B8-A04A-4761-A135-D85C5C9776F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27375" windowHeight="16440" xr2:uid="{FAC80037-6401-4965-8033-1F14E7B30D41}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="9720" xr2:uid="{FAC80037-6401-4965-8033-1F14E7B30D41}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Generated : [ Timestamp]</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>30 CPM</t>
+  </si>
+  <si>
+    <t>System Provided</t>
   </si>
 </sst>
 </file>
@@ -463,9 +466,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EDFBC8C-9A53-44CE-B471-03CE0ACB81AE}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,8 +482,7 @@
     <col min="7" max="8" width="37.7109375" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" customWidth="1"/>
     <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" customWidth="1"/>
-    <col min="12" max="12" width="13" customWidth="1"/>
+    <col min="11" max="12" width="16" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -492,6 +494,14 @@
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -552,5 +562,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>